<commit_message>
Make patches spreadsheet nicer
</commit_message>
<xml_diff>
--- a/patches/Juno60.xlsx
+++ b/patches/Juno60.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\junox\patches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73468F-9132-4C34-9285-6EBF3A1B5811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C9DB17-1574-40CD-A9C4-DDAA580B93C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16428" yWindow="-5220" windowWidth="12900" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25164" yWindow="-3840" windowWidth="19872" windowHeight="12468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank A (from service manual)" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bank A (from service manual)'!$A$1:$AA$57</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -314,15 +317,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -330,12 +339,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,6 +370,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -667,105 +695,122 @@
   <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5418,6 +5463,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AA57" xr:uid="{F3C0AD35-EBA0-4FCF-BBC0-5C497CCDE899}"/>
   <hyperlinks>
     <hyperlink ref="B57" r:id="rId1" display="https://www.synthmania.com/Roland Juno-60/Audio/Factory presets group 1/78 Synthesizer Drum.mp3" xr:uid="{9636CD77-8484-489B-9D80-1CB24DA3CEB5}"/>
     <hyperlink ref="B56" r:id="rId2" display="https://www.synthmania.com/Roland Juno-60/Audio/Factory presets group 1/77 Surf.mp3" xr:uid="{B14B3E1D-C014-4DB1-ADAA-FFF744BB72A5}"/>

</xml_diff>

<commit_message>
Improvements to patch accuracy
</commit_message>
<xml_diff>
--- a/patches/Juno60.xlsx
+++ b/patches/Juno60.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\junox\patches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EF1C50-65B3-4D7E-B59F-AAF692E4DA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E14239-3AF5-4177-9481-10FC951E50F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16284" yWindow="-5340" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bank A (from service manual)'!$A$1:$AB$57</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -333,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,12 +353,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -396,7 +400,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -722,7 +726,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5170,19 +5174,19 @@
       <c r="I52" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J52" s="1">
-        <v>0</v>
-      </c>
-      <c r="K52" s="1">
-        <v>0</v>
-      </c>
-      <c r="L52" s="1">
-        <v>0</v>
-      </c>
-      <c r="M52" s="1">
-        <v>0</v>
-      </c>
-      <c r="N52" s="1">
+      <c r="J52" s="8">
+        <v>0</v>
+      </c>
+      <c r="K52" s="8">
+        <v>0</v>
+      </c>
+      <c r="L52" s="8">
+        <v>0</v>
+      </c>
+      <c r="M52" s="8">
+        <v>0</v>
+      </c>
+      <c r="N52" s="8">
         <v>2</v>
       </c>
       <c r="O52" s="1">
@@ -5342,19 +5346,19 @@
       <c r="I54" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J54" s="1">
-        <v>0</v>
-      </c>
-      <c r="K54" s="1">
-        <v>0</v>
-      </c>
-      <c r="L54" s="1">
-        <v>0</v>
-      </c>
-      <c r="M54" s="1">
-        <v>0</v>
-      </c>
-      <c r="N54" s="1">
+      <c r="J54" s="8">
+        <v>0</v>
+      </c>
+      <c r="K54" s="8">
+        <v>0</v>
+      </c>
+      <c r="L54" s="8">
+        <v>0</v>
+      </c>
+      <c r="M54" s="8">
+        <v>0</v>
+      </c>
+      <c r="N54" s="8">
         <v>2</v>
       </c>
       <c r="O54" s="1">
@@ -5428,19 +5432,19 @@
       <c r="I55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J55" s="1">
-        <v>0</v>
-      </c>
-      <c r="K55" s="1">
-        <v>0</v>
-      </c>
-      <c r="L55" s="1">
-        <v>0</v>
-      </c>
-      <c r="M55" s="1">
-        <v>0</v>
-      </c>
-      <c r="N55" s="1">
+      <c r="J55" s="8">
+        <v>0</v>
+      </c>
+      <c r="K55" s="8">
+        <v>0</v>
+      </c>
+      <c r="L55" s="8">
+        <v>0</v>
+      </c>
+      <c r="M55" s="8">
+        <v>0</v>
+      </c>
+      <c r="N55" s="8">
         <v>2</v>
       </c>
       <c r="O55" s="1">
@@ -5514,19 +5518,19 @@
       <c r="I56" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J56" s="1">
-        <v>0</v>
-      </c>
-      <c r="K56" s="1">
-        <v>0</v>
-      </c>
-      <c r="L56" s="1">
-        <v>0</v>
-      </c>
-      <c r="M56" s="1">
-        <v>10</v>
-      </c>
-      <c r="N56" s="1">
+      <c r="J56" s="8">
+        <v>0</v>
+      </c>
+      <c r="K56" s="8">
+        <v>0</v>
+      </c>
+      <c r="L56" s="8">
+        <v>0</v>
+      </c>
+      <c r="M56" s="8">
+        <v>10</v>
+      </c>
+      <c r="N56" s="8">
         <v>10</v>
       </c>
       <c r="O56" s="1">

</xml_diff>